<commit_message>
newly Modified Reg iExam TC's
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -20,42 +20,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>iEX_TC_ID_97,iEX_TC_ID_98,iEX_TC_ID_99,iEX_TC_ID_101,iEX_TC_ID_102,iEX_TC_ID_103,iEX_TC_ID_105</t>
-  </si>
-  <si>
-    <t>@iExamRegression Validation of each component for all type of questions in Candidate flow.</t>
-  </si>
-  <si>
-    <t>failed</t>
-  </si>
-  <si>
-    <t>iEX_TC_ID_54</t>
-  </si>
-  <si>
-    <t>@iExamRegression Validation of Exam section page.</t>
-  </si>
-  <si>
-    <t>passed</t>
-  </si>
-  <si>
-    <t>iEX_TC_ID_61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@iExamRegression Validation of Exam Section &gt; Font Size </t>
-  </si>
-  <si>
-    <t>iEX_TC_ID_64</t>
-  </si>
-  <si>
-    <t>@iExamRegression Validation of Exam Section &gt; Highlighter tool highlights save scenario 1</t>
-  </si>
-  <si>
-    <t>iEX_TC_ID_76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@iExamRegression Validation of Exam section &gt; Candidate attend the exam in normal flow </t>
   </si>
 </sst>
 </file>
@@ -432,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -446,83 +410,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
newly added APIs TCs
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -22,18 +22,70 @@
     <t>Status</t>
   </si>
   <si>
-    <t>iAU_TC_ID_142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@RegressionA "Validation of Choose Question
-Scenario- 5 -
-Add 2x sessions (with duplicate sections)"</t>
+    <t>AL_001</t>
+  </si>
+  <si>
+    <t>@API Admin Login Success with Mandatory Fields</t>
   </si>
   <si>
     <t>passed</t>
   </si>
   <si>
-    <t>iAU_TC_ID_142B</t>
+    <t>QS_067</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE-CASE question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_068</t>
+  </si>
+  <si>
+    <t>@API Validation of edit ISAWE-CASE question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_069</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE-CASE question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_070</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE-CASE question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_069A</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE-CASE question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_071</t>
+  </si>
+  <si>
+    <t>@API ISAWE-CASE endpoint validation</t>
+  </si>
+  <si>
+    <t>QS_072</t>
+  </si>
+  <si>
+    <t>@API ISAWE-CASE Method validation-  incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>QS_073</t>
+  </si>
+  <si>
+    <t>@API ISAWE-CASE Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>QS_074</t>
+  </si>
+  <si>
+    <t>@API Validation of empty title field for ISAWE-CASE</t>
+  </si>
+  <si>
+    <t>failed</t>
   </si>
 </sst>
 </file>
@@ -410,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -440,10 +492,98 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
newly modified APIs TCs
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="337">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -22,24 +22,78 @@
     <t>Status</t>
   </si>
   <si>
+    <t>AL_001</t>
+  </si>
+  <si>
+    <t>@API Admin Login Success with Mandatory Fields</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>ES_001</t>
+  </si>
+  <si>
+    <t>@API Validation of Exam creation successfull message.</t>
+  </si>
+  <si>
+    <t>ES_002</t>
+  </si>
+  <si>
+    <t>@API Validation of Exam section and add questions successfull message.</t>
+  </si>
+  <si>
+    <t>ES_003</t>
+  </si>
+  <si>
+    <t>@API Validation of Approved Exam  successfull message.</t>
+  </si>
+  <si>
+    <t>ES_004</t>
+  </si>
+  <si>
+    <t>@API Validation of add user successful message.</t>
+  </si>
+  <si>
+    <t>ES_005</t>
+  </si>
+  <si>
+    <t>@API Validation of Empty Exam name field in Exam Page.</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>ES_006</t>
+  </si>
+  <si>
+    <t>@API Exam creation-endpoint validation</t>
+  </si>
+  <si>
+    <t>ES_007</t>
+  </si>
+  <si>
+    <t>@API Exam creation-Method validation-  incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>ES_008</t>
+  </si>
+  <si>
+    <t>@API Exam creation-Header field validation - invalid</t>
+  </si>
+  <si>
     <t>CS_001</t>
   </si>
   <si>
     <t>@API Candidate Login Success with Mandatory Fields</t>
   </si>
   <si>
-    <t>passed</t>
-  </si>
-  <si>
     <t>CS_013</t>
   </si>
   <si>
     <t>@API candidate dashboard Header field validation - invalid</t>
   </si>
   <si>
-    <t>failed</t>
-  </si>
-  <si>
     <t>CS_002</t>
   </si>
   <si>
@@ -446,6 +500,528 @@
   </si>
   <si>
     <t>@API candidate chat setting endpoint validation</t>
+  </si>
+  <si>
+    <t>QS_067</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE-CASE question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_068</t>
+  </si>
+  <si>
+    <t>@API Validation of edit ISAWE-CASE question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_069</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE-CASE question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_070</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE-CASE question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_069A</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE-CASE question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_071</t>
+  </si>
+  <si>
+    <t>@API ISAWE-CASE endpoint validation</t>
+  </si>
+  <si>
+    <t>QS_072</t>
+  </si>
+  <si>
+    <t>@API ISAWE-CASE Method validation-  incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>QS_073</t>
+  </si>
+  <si>
+    <t>@API ISAWE-CASE Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>QS_074</t>
+  </si>
+  <si>
+    <t>@API Validation of empty title field for ISAWE-CASE</t>
+  </si>
+  <si>
+    <t>QS_035</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_036</t>
+  </si>
+  <si>
+    <t>@API Validation of edit ISAWE question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_037</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_038</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_037A</t>
+  </si>
+  <si>
+    <t>@API Validation of ISAWE question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_039</t>
+  </si>
+  <si>
+    <t>@API endpoint validation</t>
+  </si>
+  <si>
+    <t>QS_040</t>
+  </si>
+  <si>
+    <t>@API Method validation-  incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>QS_041</t>
+  </si>
+  <si>
+    <t>@API Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>QS_042</t>
+  </si>
+  <si>
+    <t>@API Validation of empty title field.</t>
+  </si>
+  <si>
+    <t>QS_001</t>
+  </si>
+  <si>
+    <t>@API Validation of MCQ question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_002</t>
+  </si>
+  <si>
+    <t>@API Validation of edit MCQ question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_003</t>
+  </si>
+  <si>
+    <t>@API Validation of MCQ question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_005</t>
+  </si>
+  <si>
+    <t>@API Validation of MCQ question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_003A</t>
+  </si>
+  <si>
+    <t>@API Validation of MCQ question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_004</t>
+  </si>
+  <si>
+    <t>@API Validation of create question page.</t>
+  </si>
+  <si>
+    <t>QS_006</t>
+  </si>
+  <si>
+    <t>QS_007</t>
+  </si>
+  <si>
+    <t>QS_008</t>
+  </si>
+  <si>
+    <t>QS_009</t>
+  </si>
+  <si>
+    <t>QS_107</t>
+  </si>
+  <si>
+    <t>@API Validation of Ranking question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_108</t>
+  </si>
+  <si>
+    <t>@API Validation of edit Ranking question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_109</t>
+  </si>
+  <si>
+    <t>@API Validation of Ranking question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_110</t>
+  </si>
+  <si>
+    <t>@API Validation of Ranking question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_109A</t>
+  </si>
+  <si>
+    <t>@API Validation of Ranking question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_111</t>
+  </si>
+  <si>
+    <t>@API Ranking question endpoint validation</t>
+  </si>
+  <si>
+    <t>QS_112</t>
+  </si>
+  <si>
+    <t>@API Ranking question Method validation-  incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>QS_113</t>
+  </si>
+  <si>
+    <t>@API Ranking question Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>QS_114</t>
+  </si>
+  <si>
+    <t>@API Validation of empty title field for Ranking question</t>
+  </si>
+  <si>
+    <t>QS_010</t>
+  </si>
+  <si>
+    <t>@API Validation of SAQ question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_011</t>
+  </si>
+  <si>
+    <t>@API Validation of edit SAQ question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_012</t>
+  </si>
+  <si>
+    <t>@API Validation of SAQ question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_014</t>
+  </si>
+  <si>
+    <t>@API Validation of SAQ question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_012A</t>
+  </si>
+  <si>
+    <t>@API Validation of SAQ question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_015</t>
+  </si>
+  <si>
+    <t>QS_016</t>
+  </si>
+  <si>
+    <t>QS_017</t>
+  </si>
+  <si>
+    <t>QS_018</t>
+  </si>
+  <si>
+    <t>QS_059</t>
+  </si>
+  <si>
+    <t>@API Validation of Scenario question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_060</t>
+  </si>
+  <si>
+    <t>@API Validation of edit Scenario question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_061</t>
+  </si>
+  <si>
+    <t>@API Validation of Scenario question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_062</t>
+  </si>
+  <si>
+    <t>@API Validation of Scenario question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_061A</t>
+  </si>
+  <si>
+    <t>@API Validation of Scenario question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_063</t>
+  </si>
+  <si>
+    <t>@API Scenario question endpoint validation</t>
+  </si>
+  <si>
+    <t>QS_064</t>
+  </si>
+  <si>
+    <t>@API Scenario question- Method validation-  incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>QS_065</t>
+  </si>
+  <si>
+    <t>@API Scenario question- Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>QS_066</t>
+  </si>
+  <si>
+    <t>@API Validation of empty title field for Scenario question</t>
+  </si>
+  <si>
+    <t>QS_051</t>
+  </si>
+  <si>
+    <t>@API Validation of SJT question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_052</t>
+  </si>
+  <si>
+    <t>@API Validation of edit SJT question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_053</t>
+  </si>
+  <si>
+    <t>@API Validation of SJT question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_054</t>
+  </si>
+  <si>
+    <t>@API Validation of SJT question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_053A</t>
+  </si>
+  <si>
+    <t>@API Validation of SJT question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_055</t>
+  </si>
+  <si>
+    <t>QS_056</t>
+  </si>
+  <si>
+    <t>QS_057</t>
+  </si>
+  <si>
+    <t>QS_058</t>
+  </si>
+  <si>
+    <t>QS_027</t>
+  </si>
+  <si>
+    <t>@API Validation of Type-B question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_028</t>
+  </si>
+  <si>
+    <t>@API Validation of edit Type-B question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_029</t>
+  </si>
+  <si>
+    <t>@API Validation of Type-B question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_030</t>
+  </si>
+  <si>
+    <t>@API Validation of Type-B question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_029A</t>
+  </si>
+  <si>
+    <t>@API Validation of Type-B question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_031</t>
+  </si>
+  <si>
+    <t>QS_032</t>
+  </si>
+  <si>
+    <t>QS_033</t>
+  </si>
+  <si>
+    <t>QS_034</t>
+  </si>
+  <si>
+    <t>QS_043</t>
+  </si>
+  <si>
+    <t>@API Validation of Type-X question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_044</t>
+  </si>
+  <si>
+    <t>@API Validation of edit Type-X question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_045</t>
+  </si>
+  <si>
+    <t>@API Validation of Type-X question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_046</t>
+  </si>
+  <si>
+    <t>@API Validation of Type-X question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_045A</t>
+  </si>
+  <si>
+    <t>@API Validation of Type-X question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_047</t>
+  </si>
+  <si>
+    <t>QS_048</t>
+  </si>
+  <si>
+    <t>QS_049</t>
+  </si>
+  <si>
+    <t>QS_050</t>
+  </si>
+  <si>
+    <t>QS_019</t>
+  </si>
+  <si>
+    <t>@API Validation of VSAQ question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_020</t>
+  </si>
+  <si>
+    <t>@API Validation of edit VSAQ question successfull message.</t>
+  </si>
+  <si>
+    <t>QS_021</t>
+  </si>
+  <si>
+    <t>@API Validation of VSAQ question Approved message.</t>
+  </si>
+  <si>
+    <t>QS_022</t>
+  </si>
+  <si>
+    <t>@API Validation of VSAQ question checkout message.</t>
+  </si>
+  <si>
+    <t>QS_021A</t>
+  </si>
+  <si>
+    <t>@API Validation of VSAQ question Approved message (again).</t>
+  </si>
+  <si>
+    <t>QS_023</t>
+  </si>
+  <si>
+    <t>QS_024</t>
+  </si>
+  <si>
+    <t>QS_025</t>
+  </si>
+  <si>
+    <t>QS_026</t>
+  </si>
+  <si>
+    <t>AL_002</t>
+  </si>
+  <si>
+    <t>@API To verify the response when passing an invalid endpoint.</t>
+  </si>
+  <si>
+    <t>AL_003</t>
+  </si>
+  <si>
+    <t>@API To verify the response when an incorrect HTTP method is used for a request.</t>
+  </si>
+  <si>
+    <t>AL_004</t>
+  </si>
+  <si>
+    <t>@API To verify the response on passing invalid webreferer in the header field.</t>
+  </si>
+  <si>
+    <t>AL_005</t>
+  </si>
+  <si>
+    <t>@API To verify the response on passing empty webreferer in the header field.</t>
+  </si>
+  <si>
+    <t>AL_006</t>
+  </si>
+  <si>
+    <t>@API To verify the response on passing invalid username in the request field.</t>
+  </si>
+  <si>
+    <t>AL_007</t>
+  </si>
+  <si>
+    <t>@API To verify the response on passing empty username in the request field.</t>
+  </si>
+  <si>
+    <t>AL_008</t>
+  </si>
+  <si>
+    <t>@API To verify the response on passing invalid password in the request field.</t>
+  </si>
+  <si>
+    <t>AL_009</t>
+  </si>
+  <si>
+    <t>@API To verify the response on passing empty password in the request field.</t>
   </si>
 </sst>
 </file>
@@ -822,7 +1398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C193"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -849,21 +1425,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -871,10 +1447,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -882,76 +1458,76 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -959,21 +1535,21 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -981,10 +1557,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -992,24 +1568,24 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,51 +1593,51 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1069,21 +1645,21 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1091,10 +1667,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -1102,21 +1678,21 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1124,10 +1700,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1135,10 +1711,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -1146,32 +1722,32 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -1182,7 +1758,7 @@
         <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1190,10 +1766,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1201,10 +1777,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -1212,10 +1788,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -1223,10 +1799,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1234,10 +1810,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -1245,10 +1821,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -1256,10 +1832,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1267,10 +1843,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1278,10 +1854,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1289,10 +1865,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -1300,10 +1876,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -1311,10 +1887,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1322,10 +1898,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1333,10 +1909,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1344,10 +1920,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1355,10 +1931,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1366,10 +1942,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -1377,10 +1953,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1388,10 +1964,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1399,10 +1975,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1410,10 +1986,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1421,10 +1997,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -1432,10 +2008,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1443,10 +2019,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1454,10 +2030,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -1465,10 +2041,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1476,10 +2052,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1487,10 +2063,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1498,10 +2074,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1509,10 +2085,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -1520,10 +2096,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -1531,10 +2107,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -1542,10 +2118,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -1553,10 +2129,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -1564,10 +2140,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -1575,10 +2151,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -1586,10 +2162,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -1597,10 +2173,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -1608,10 +2184,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -1619,10 +2195,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
@@ -1630,13 +2206,1322 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>143</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>144</v>
       </c>
-      <c r="C74" t="s">
-        <v>5</v>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" t="s">
+        <v>148</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>149</v>
+      </c>
+      <c r="B78" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>151</v>
+      </c>
+      <c r="B79" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>153</v>
+      </c>
+      <c r="B80" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>155</v>
+      </c>
+      <c r="B81" t="s">
+        <v>156</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" t="s">
+        <v>164</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>165</v>
+      </c>
+      <c r="B87" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>167</v>
+      </c>
+      <c r="B88" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>169</v>
+      </c>
+      <c r="B89" t="s">
+        <v>170</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>171</v>
+      </c>
+      <c r="B90" t="s">
+        <v>172</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>173</v>
+      </c>
+      <c r="B91" t="s">
+        <v>174</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>175</v>
+      </c>
+      <c r="B92" t="s">
+        <v>176</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>177</v>
+      </c>
+      <c r="B93" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>181</v>
+      </c>
+      <c r="B96" t="s">
+        <v>182</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>183</v>
+      </c>
+      <c r="B97" t="s">
+        <v>184</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>185</v>
+      </c>
+      <c r="B98" t="s">
+        <v>186</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>187</v>
+      </c>
+      <c r="B99" t="s">
+        <v>188</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>189</v>
+      </c>
+      <c r="B100" t="s">
+        <v>190</v>
+      </c>
+      <c r="C100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>191</v>
+      </c>
+      <c r="B101" t="s">
+        <v>192</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>193</v>
+      </c>
+      <c r="B102" t="s">
+        <v>194</v>
+      </c>
+      <c r="C102" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>195</v>
+      </c>
+      <c r="B103" t="s">
+        <v>196</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>197</v>
+      </c>
+      <c r="B104" t="s">
+        <v>198</v>
+      </c>
+      <c r="C104" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105" t="s">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>199</v>
+      </c>
+      <c r="B106" t="s">
+        <v>200</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>201</v>
+      </c>
+      <c r="B107" t="s">
+        <v>202</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>203</v>
+      </c>
+      <c r="B108" t="s">
+        <v>204</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>205</v>
+      </c>
+      <c r="B109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>207</v>
+      </c>
+      <c r="B110" t="s">
+        <v>208</v>
+      </c>
+      <c r="C110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>209</v>
+      </c>
+      <c r="B111" t="s">
+        <v>210</v>
+      </c>
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>211</v>
+      </c>
+      <c r="B112" t="s">
+        <v>192</v>
+      </c>
+      <c r="C112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>212</v>
+      </c>
+      <c r="B113" t="s">
+        <v>194</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>213</v>
+      </c>
+      <c r="B114" t="s">
+        <v>196</v>
+      </c>
+      <c r="C114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>214</v>
+      </c>
+      <c r="B115" t="s">
+        <v>198</v>
+      </c>
+      <c r="C115" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" t="s">
+        <v>4</v>
+      </c>
+      <c r="C116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>215</v>
+      </c>
+      <c r="B117" t="s">
+        <v>216</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>217</v>
+      </c>
+      <c r="B118" t="s">
+        <v>218</v>
+      </c>
+      <c r="C118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>219</v>
+      </c>
+      <c r="B119" t="s">
+        <v>220</v>
+      </c>
+      <c r="C119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>221</v>
+      </c>
+      <c r="B120" t="s">
+        <v>222</v>
+      </c>
+      <c r="C120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>223</v>
+      </c>
+      <c r="B121" t="s">
+        <v>224</v>
+      </c>
+      <c r="C121" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>225</v>
+      </c>
+      <c r="B122" t="s">
+        <v>226</v>
+      </c>
+      <c r="C122" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>227</v>
+      </c>
+      <c r="B123" t="s">
+        <v>228</v>
+      </c>
+      <c r="C123" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>229</v>
+      </c>
+      <c r="B124" t="s">
+        <v>230</v>
+      </c>
+      <c r="C124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>231</v>
+      </c>
+      <c r="B125" t="s">
+        <v>232</v>
+      </c>
+      <c r="C125" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>3</v>
+      </c>
+      <c r="B126" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>233</v>
+      </c>
+      <c r="B127" t="s">
+        <v>234</v>
+      </c>
+      <c r="C127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>235</v>
+      </c>
+      <c r="B128" t="s">
+        <v>236</v>
+      </c>
+      <c r="C128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>237</v>
+      </c>
+      <c r="B129" t="s">
+        <v>238</v>
+      </c>
+      <c r="C129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>239</v>
+      </c>
+      <c r="B130" t="s">
+        <v>240</v>
+      </c>
+      <c r="C130" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>241</v>
+      </c>
+      <c r="B131" t="s">
+        <v>242</v>
+      </c>
+      <c r="C131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>243</v>
+      </c>
+      <c r="B132" t="s">
+        <v>192</v>
+      </c>
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>244</v>
+      </c>
+      <c r="B133" t="s">
+        <v>194</v>
+      </c>
+      <c r="C133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>245</v>
+      </c>
+      <c r="B134" t="s">
+        <v>196</v>
+      </c>
+      <c r="C134" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>246</v>
+      </c>
+      <c r="B135" t="s">
+        <v>198</v>
+      </c>
+      <c r="C135" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>247</v>
+      </c>
+      <c r="B137" t="s">
+        <v>248</v>
+      </c>
+      <c r="C137" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>249</v>
+      </c>
+      <c r="B138" t="s">
+        <v>250</v>
+      </c>
+      <c r="C138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>251</v>
+      </c>
+      <c r="B139" t="s">
+        <v>252</v>
+      </c>
+      <c r="C139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>253</v>
+      </c>
+      <c r="B140" t="s">
+        <v>254</v>
+      </c>
+      <c r="C140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>255</v>
+      </c>
+      <c r="B141" t="s">
+        <v>256</v>
+      </c>
+      <c r="C141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>257</v>
+      </c>
+      <c r="B142" t="s">
+        <v>258</v>
+      </c>
+      <c r="C142" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>259</v>
+      </c>
+      <c r="B143" t="s">
+        <v>260</v>
+      </c>
+      <c r="C143" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>261</v>
+      </c>
+      <c r="B144" t="s">
+        <v>262</v>
+      </c>
+      <c r="C144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>263</v>
+      </c>
+      <c r="B145" t="s">
+        <v>264</v>
+      </c>
+      <c r="C145" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>265</v>
+      </c>
+      <c r="B147" t="s">
+        <v>266</v>
+      </c>
+      <c r="C147" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>267</v>
+      </c>
+      <c r="B148" t="s">
+        <v>268</v>
+      </c>
+      <c r="C148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>269</v>
+      </c>
+      <c r="B149" t="s">
+        <v>270</v>
+      </c>
+      <c r="C149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>271</v>
+      </c>
+      <c r="B150" t="s">
+        <v>272</v>
+      </c>
+      <c r="C150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>273</v>
+      </c>
+      <c r="B151" t="s">
+        <v>274</v>
+      </c>
+      <c r="C151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>275</v>
+      </c>
+      <c r="B152" t="s">
+        <v>192</v>
+      </c>
+      <c r="C152" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>276</v>
+      </c>
+      <c r="B153" t="s">
+        <v>194</v>
+      </c>
+      <c r="C153" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>277</v>
+      </c>
+      <c r="B154" t="s">
+        <v>196</v>
+      </c>
+      <c r="C154" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>278</v>
+      </c>
+      <c r="B155" t="s">
+        <v>198</v>
+      </c>
+      <c r="C155" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>3</v>
+      </c>
+      <c r="B156" t="s">
+        <v>4</v>
+      </c>
+      <c r="C156" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>279</v>
+      </c>
+      <c r="B157" t="s">
+        <v>280</v>
+      </c>
+      <c r="C157" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>281</v>
+      </c>
+      <c r="B158" t="s">
+        <v>282</v>
+      </c>
+      <c r="C158" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>283</v>
+      </c>
+      <c r="B159" t="s">
+        <v>284</v>
+      </c>
+      <c r="C159" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>285</v>
+      </c>
+      <c r="B160" t="s">
+        <v>286</v>
+      </c>
+      <c r="C160" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>287</v>
+      </c>
+      <c r="B161" t="s">
+        <v>288</v>
+      </c>
+      <c r="C161" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>289</v>
+      </c>
+      <c r="B162" t="s">
+        <v>192</v>
+      </c>
+      <c r="C162" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>290</v>
+      </c>
+      <c r="B163" t="s">
+        <v>194</v>
+      </c>
+      <c r="C163" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>291</v>
+      </c>
+      <c r="B164" t="s">
+        <v>196</v>
+      </c>
+      <c r="C164" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>292</v>
+      </c>
+      <c r="B165" t="s">
+        <v>198</v>
+      </c>
+      <c r="C165" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" t="s">
+        <v>4</v>
+      </c>
+      <c r="C166" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>293</v>
+      </c>
+      <c r="B167" t="s">
+        <v>294</v>
+      </c>
+      <c r="C167" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>295</v>
+      </c>
+      <c r="B168" t="s">
+        <v>296</v>
+      </c>
+      <c r="C168" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>297</v>
+      </c>
+      <c r="B169" t="s">
+        <v>298</v>
+      </c>
+      <c r="C169" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>299</v>
+      </c>
+      <c r="B170" t="s">
+        <v>300</v>
+      </c>
+      <c r="C170" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>301</v>
+      </c>
+      <c r="B171" t="s">
+        <v>302</v>
+      </c>
+      <c r="C171" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>303</v>
+      </c>
+      <c r="B172" t="s">
+        <v>192</v>
+      </c>
+      <c r="C172" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>304</v>
+      </c>
+      <c r="B173" t="s">
+        <v>194</v>
+      </c>
+      <c r="C173" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>305</v>
+      </c>
+      <c r="B174" t="s">
+        <v>196</v>
+      </c>
+      <c r="C174" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>306</v>
+      </c>
+      <c r="B175" t="s">
+        <v>198</v>
+      </c>
+      <c r="C175" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>3</v>
+      </c>
+      <c r="B176" t="s">
+        <v>4</v>
+      </c>
+      <c r="C176" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>307</v>
+      </c>
+      <c r="B177" t="s">
+        <v>308</v>
+      </c>
+      <c r="C177" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>309</v>
+      </c>
+      <c r="B178" t="s">
+        <v>310</v>
+      </c>
+      <c r="C178" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>311</v>
+      </c>
+      <c r="B179" t="s">
+        <v>312</v>
+      </c>
+      <c r="C179" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>313</v>
+      </c>
+      <c r="B180" t="s">
+        <v>314</v>
+      </c>
+      <c r="C180" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>315</v>
+      </c>
+      <c r="B181" t="s">
+        <v>316</v>
+      </c>
+      <c r="C181" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>317</v>
+      </c>
+      <c r="B182" t="s">
+        <v>192</v>
+      </c>
+      <c r="C182" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>318</v>
+      </c>
+      <c r="B183" t="s">
+        <v>194</v>
+      </c>
+      <c r="C183" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>319</v>
+      </c>
+      <c r="B184" t="s">
+        <v>196</v>
+      </c>
+      <c r="C184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>320</v>
+      </c>
+      <c r="B185" t="s">
+        <v>198</v>
+      </c>
+      <c r="C185" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>321</v>
+      </c>
+      <c r="B186" t="s">
+        <v>322</v>
+      </c>
+      <c r="C186" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>323</v>
+      </c>
+      <c r="B187" t="s">
+        <v>324</v>
+      </c>
+      <c r="C187" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>325</v>
+      </c>
+      <c r="B188" t="s">
+        <v>326</v>
+      </c>
+      <c r="C188" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>327</v>
+      </c>
+      <c r="B189" t="s">
+        <v>328</v>
+      </c>
+      <c r="C189" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>329</v>
+      </c>
+      <c r="B190" t="s">
+        <v>330</v>
+      </c>
+      <c r="C190" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>331</v>
+      </c>
+      <c r="B191" t="s">
+        <v>332</v>
+      </c>
+      <c r="C191" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>333</v>
+      </c>
+      <c r="B192" t="s">
+        <v>334</v>
+      </c>
+      <c r="C192" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>335</v>
+      </c>
+      <c r="B193" t="s">
+        <v>336</v>
+      </c>
+      <c r="C193" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
newly added few more commom setting APIs TCs
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="281">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -622,13 +622,70 @@
     <t>@API Admin delete-role_validation of incorrect HTTP method</t>
   </si>
   <si>
+    <t>Admin_128</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the user-activities-filter</t>
+  </si>
+  <si>
+    <t>Admin_129</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for user-activities-filter</t>
+  </si>
+  <si>
+    <t>Admin_131</t>
+  </si>
+  <si>
+    <t>@API Admin_user-activities-list</t>
+  </si>
+  <si>
+    <t>Admin_132</t>
+  </si>
+  <si>
+    <t>@API Admin user-activities-list_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_133</t>
+  </si>
+  <si>
+    <t>@API Admin user-activities-list_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_134</t>
+  </si>
+  <si>
+    <t>@API Admin_user-activities-list-pagination</t>
+  </si>
+  <si>
+    <t>Admin_135</t>
+  </si>
+  <si>
+    <t>@API Admin user-activities-list-pagination_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_136</t>
+  </si>
+  <si>
+    <t>@API Admin user-activities-list-pagination_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_0130</t>
+  </si>
+  <si>
+    <t>@API Admin user-activities-filter-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>AL_001T</t>
+  </si>
+  <si>
     <t>Admin_090</t>
   </si>
   <si>
     <t>@API Admin delete-role-Header field validation - invalid</t>
-  </si>
-  <si>
-    <t>failed</t>
   </si>
   <si>
     <t>AL_001S</t>
@@ -1173,7 +1230,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C142"/>
+  <dimension ref="A1:C152"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2317,15 +2374,15 @@
         <v>204</v>
       </c>
       <c r="C104" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105" t="s">
         <v>206</v>
-      </c>
-      <c r="B105" t="s">
-        <v>4</v>
       </c>
       <c r="C105" t="s">
         <v>5</v>
@@ -2339,7 +2396,7 @@
         <v>208</v>
       </c>
       <c r="C106" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2347,7 +2404,7 @@
         <v>209</v>
       </c>
       <c r="B107" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
@@ -2355,21 +2412,21 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B108" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C108" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>214</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
@@ -2377,21 +2434,21 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B110" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C110" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>218</v>
       </c>
       <c r="C111" t="s">
         <v>5</v>
@@ -2399,18 +2456,18 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B112" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C112" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B113" t="s">
         <v>4</v>
@@ -2421,18 +2478,18 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B114" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C114" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B115" t="s">
         <v>4</v>
@@ -2443,18 +2500,18 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B116" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C116" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B117" t="s">
         <v>4</v>
@@ -2465,18 +2522,18 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B118" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C118" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B119" t="s">
         <v>4</v>
@@ -2487,18 +2544,18 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B120" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C120" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B121" t="s">
         <v>4</v>
@@ -2509,40 +2566,40 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B122" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C122" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B123" t="s">
         <v>4</v>
       </c>
       <c r="C123" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B124" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C124" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B125" t="s">
         <v>4</v>
@@ -2553,18 +2610,18 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B126" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C126" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B127" t="s">
         <v>4</v>
@@ -2575,18 +2632,18 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B128" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C128" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B129" t="s">
         <v>4</v>
@@ -2597,18 +2654,18 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B130" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C130" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B131" t="s">
         <v>4</v>
@@ -2619,18 +2676,18 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B132" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C132" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B133" t="s">
         <v>4</v>
@@ -2641,18 +2698,18 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B134" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C134" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B135" t="s">
         <v>4</v>
@@ -2663,18 +2720,18 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B136" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C136" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B137" t="s">
         <v>4</v>
@@ -2685,18 +2742,18 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B138" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C138" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B139" t="s">
         <v>4</v>
@@ -2707,18 +2764,18 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B140" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C140" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B141" t="s">
         <v>4</v>
@@ -2729,13 +2786,123 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B142" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C142" t="s">
-        <v>205</v>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>266</v>
+      </c>
+      <c r="B143" t="s">
+        <v>4</v>
+      </c>
+      <c r="C143" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>267</v>
+      </c>
+      <c r="B144" t="s">
+        <v>268</v>
+      </c>
+      <c r="C144" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>269</v>
+      </c>
+      <c r="B145" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>270</v>
+      </c>
+      <c r="B146" t="s">
+        <v>271</v>
+      </c>
+      <c r="C146" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>272</v>
+      </c>
+      <c r="B147" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>273</v>
+      </c>
+      <c r="B148" t="s">
+        <v>274</v>
+      </c>
+      <c r="C148" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>275</v>
+      </c>
+      <c r="B149" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>276</v>
+      </c>
+      <c r="B150" t="s">
+        <v>277</v>
+      </c>
+      <c r="C150" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>278</v>
+      </c>
+      <c r="B151" t="s">
+        <v>4</v>
+      </c>
+      <c r="C151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>279</v>
+      </c>
+      <c r="B152" t="s">
+        <v>280</v>
+      </c>
+      <c r="C152" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
common setting remaining tc's added
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="746">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -337,19 +337,19 @@
     <t>Admin_070</t>
   </si>
   <si>
-    <t>@API Admin_users-search</t>
+    <t>@API Admin_users-login</t>
   </si>
   <si>
     <t>Admin_071</t>
   </si>
   <si>
-    <t>@API Admin users-search_validation of incorrect HTTP method</t>
+    <t>@API Admin users-login_validation of incorrect HTTP method</t>
   </si>
   <si>
     <t>Admin_072</t>
   </si>
   <si>
-    <t>@API Admin users-search_validation of invalid endpoint.</t>
+    <t>@API Admin users-login_validation of invalid endpoint.</t>
   </si>
   <si>
     <t>Admin_076</t>
@@ -754,13 +754,1315 @@
     <t>@API Admin custom-filter-save public or privet_validation of invalid endpoint.</t>
   </si>
   <si>
+    <t>Admin_146</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the email-template-create-form</t>
+  </si>
+  <si>
+    <t>Admin_147</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for email-template-create-form</t>
+  </si>
+  <si>
+    <t>Admin_149</t>
+  </si>
+  <si>
+    <t>@API Admin_email-template-save</t>
+  </si>
+  <si>
+    <t>Admin_150</t>
+  </si>
+  <si>
+    <t>@API Admin email-template-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_151</t>
+  </si>
+  <si>
+    <t>@API Admin email-template-save_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_158</t>
+  </si>
+  <si>
+    <t>@API Admin_email-templates-list</t>
+  </si>
+  <si>
+    <t>Admin_159</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-list_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_160</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-list_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_161</t>
+  </si>
+  <si>
+    <t>@API Admin_email-templates-search</t>
+  </si>
+  <si>
+    <t>Admin_162</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-searcht_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_163</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_164</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the email-template-filter-list</t>
+  </si>
+  <si>
+    <t>Admin_165</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for email-template-filter-list</t>
+  </si>
+  <si>
+    <t>Admin_167</t>
+  </si>
+  <si>
+    <t>@API Admin_email-templates-pagination</t>
+  </si>
+  <si>
+    <t>Admin_168</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-pagination_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_169</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-pagination_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_170</t>
+  </si>
+  <si>
+    <t>@API Admin_email-templates-filter-search</t>
+  </si>
+  <si>
+    <t>Admin_171</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-filter-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_172</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-filter-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_173</t>
+  </si>
+  <si>
+    <t>@API Admin_custom-filter-save</t>
+  </si>
+  <si>
+    <t>Admin_174</t>
+  </si>
+  <si>
+    <t>@API Admin custom-filter-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_175</t>
+  </si>
+  <si>
+    <t>@API Admin custom-filter-save_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_176</t>
+  </si>
+  <si>
+    <t>@API Admin_email-templates-list-field-column-hide</t>
+  </si>
+  <si>
+    <t>Admin_177</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-list-field-column-hide_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_178</t>
+  </si>
+  <si>
+    <t>@API Admin email-templates-list-field-column-hide_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_152</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the email-template-edit-form</t>
+  </si>
+  <si>
+    <t>Admin_153</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for email-template-edit-form</t>
+  </si>
+  <si>
+    <t>Admin_155</t>
+  </si>
+  <si>
+    <t>@API Admin_email-template-update</t>
+  </si>
+  <si>
+    <t>Admin_156</t>
+  </si>
+  <si>
+    <t>@API Admin email-template-update_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_157</t>
+  </si>
+  <si>
+    <t>@API Admin email-template-update_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_179</t>
+  </si>
+  <si>
+    <t>@API Admin_create-dashboard-form</t>
+  </si>
+  <si>
+    <t>Admin_180</t>
+  </si>
+  <si>
+    <t>@API Admin create-dashboard-form_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_181</t>
+  </si>
+  <si>
+    <t>@API Admin_create-dashboard-save</t>
+  </si>
+  <si>
+    <t>Admin_182</t>
+  </si>
+  <si>
+    <t>@API Admin create-dashboard-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_183</t>
+  </si>
+  <si>
+    <t>@API Admin create-dashboard-save_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_184</t>
+  </si>
+  <si>
+    <t>@API Admin_dashboards-list</t>
+  </si>
+  <si>
+    <t>Admin_185</t>
+  </si>
+  <si>
+    <t>@API Admin dashboards-list_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_186</t>
+  </si>
+  <si>
+    <t>@API Admin dashboards-list_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_187</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the dashboard-filter-list</t>
+  </si>
+  <si>
+    <t>Admin_188</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for dashboard-filter-list</t>
+  </si>
+  <si>
+    <t>Admin_190</t>
+  </si>
+  <si>
+    <t>@API Admin_dashboards-search</t>
+  </si>
+  <si>
+    <t>Admin_191</t>
+  </si>
+  <si>
+    <t>@API Admin dashboards-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_192</t>
+  </si>
+  <si>
+    <t>@API Admin dashboards-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_193</t>
+  </si>
+  <si>
+    <t>@API Admin_dashboards-filter-search</t>
+  </si>
+  <si>
+    <t>Admin_194</t>
+  </si>
+  <si>
+    <t>@API Admin dashboards-filter-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_195</t>
+  </si>
+  <si>
+    <t>@API Admin dashboards-filter-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_196</t>
+  </si>
+  <si>
+    <t>@API Admin_custom-filter-save public or private</t>
+  </si>
+  <si>
+    <t>Admin_197</t>
+  </si>
+  <si>
+    <t>@API Admin custom-filter-save public or private_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_198</t>
+  </si>
+  <si>
+    <t>@API Admin custom-filter-save public or private_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_199</t>
+  </si>
+  <si>
+    <t>@API Admin_dashboards-list-field-column-hide</t>
+  </si>
+  <si>
+    <t>Admin_200</t>
+  </si>
+  <si>
+    <t>@API Admin dashboards-list-field-column-hide_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_201</t>
+  </si>
+  <si>
+    <t>@API Admin dashboards-list-field-column-hide_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_202</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the dashboard-list-status-change</t>
+  </si>
+  <si>
+    <t>Admin_204</t>
+  </si>
+  <si>
+    <t>@API Admin_edit-dashboard-form</t>
+  </si>
+  <si>
+    <t>Admin_205 @API Admin edit-dashboard-form_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_206</t>
+  </si>
+  <si>
+    <t>@API Admin_dashboard-update</t>
+  </si>
+  <si>
+    <t>Admin_207</t>
+  </si>
+  <si>
+    <t>@API Admin dashboard-update_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_208</t>
+  </si>
+  <si>
+    <t>@API Admin dashboard-update_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_209</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the duplicate-dashboard</t>
+  </si>
+  <si>
+    <t>Admin_210</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for duplicate-dashboard</t>
+  </si>
+  <si>
+    <t>Admin_212</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the delete-dashboard</t>
+  </si>
+  <si>
+    <t>Admin_213</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for delete-dashboard</t>
+  </si>
+  <si>
+    <t>Admin_215</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the chat-settings-form</t>
+  </si>
+  <si>
+    <t>Admin_216</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for chat-settings-form</t>
+  </si>
+  <si>
+    <t>Admin_218</t>
+  </si>
+  <si>
+    <t>@API Admin_chat-settings-save</t>
+  </si>
+  <si>
+    <t>Admin_219</t>
+  </si>
+  <si>
+    <t>@API Admin chat-settings-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_220</t>
+  </si>
+  <si>
+    <t>@API Admin chat-settings-save_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_221</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_centre-form</t>
+  </si>
+  <si>
+    <t>Admin_222</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for training_centre-form</t>
+  </si>
+  <si>
+    <t>Admin_224</t>
+  </si>
+  <si>
+    <t>@API Admin_training_centre-save</t>
+  </si>
+  <si>
+    <t>Admin_225</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_226</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-save_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_227</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_centre-edit-form</t>
+  </si>
+  <si>
+    <t>Admin_228</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for training_centre-edit-form</t>
+  </si>
+  <si>
+    <t>Admin_230</t>
+  </si>
+  <si>
+    <t>@API Admin_training_centre-update</t>
+  </si>
+  <si>
+    <t>Admin_231</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-update_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_232</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-update_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_233</t>
+  </si>
+  <si>
+    <t>@API Admin_training_centres-list</t>
+  </si>
+  <si>
+    <t>Admin_234</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-list_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_235</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-list_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_236</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_centres-filters</t>
+  </si>
+  <si>
+    <t>Admin_237</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for training_centres-filters</t>
+  </si>
+  <si>
+    <t>Admin_240</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_241</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_243</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-filter-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_244</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-filter-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_245</t>
+  </si>
+  <si>
+    <t>@API Admin_training_centre-custom-filter-save</t>
+  </si>
+  <si>
+    <t>Admin_246</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-custom-filter-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_247</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-custom-filter-save-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_249</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-field-column-show and hide_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_250</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-field-column-show and hide_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_252</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-pagination_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_253</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-pagination_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_254</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the deactivate_training_centre</t>
+  </si>
+  <si>
+    <t>Admin_255</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for deactivate_training_centre</t>
+  </si>
+  <si>
+    <t>Admin_257</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the activate_training_centre</t>
+  </si>
+  <si>
+    <t>Admin_258</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for activate_training_centre</t>
+  </si>
+  <si>
+    <t>Admin_260</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_centre-delete</t>
+  </si>
+  <si>
+    <t>Admin_261</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for training_centre-delete</t>
+  </si>
+  <si>
+    <t>Admin_263</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_site-form</t>
+  </si>
+  <si>
+    <t>Admin_264</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for training_site-form</t>
+  </si>
+  <si>
+    <t>Admin_266</t>
+  </si>
+  <si>
+    <t>@API Admin_training_site-save</t>
+  </si>
+  <si>
+    <t>Admin_267</t>
+  </si>
+  <si>
+    <t>@API Admin training_site-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_268</t>
+  </si>
+  <si>
+    <t>@API Admin training_site-save_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_269</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_site-edit-form</t>
+  </si>
+  <si>
+    <t>Admin_270</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for training_site-edit-form</t>
+  </si>
+  <si>
+    <t>Admin_272</t>
+  </si>
+  <si>
+    <t>@API Admin_training_sites-list</t>
+  </si>
+  <si>
+    <t>Admin_273</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-list_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_274</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-list_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_276</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_277</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_279</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-filter-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_280</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-filter-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_281</t>
+  </si>
+  <si>
+    <t>@API Admin_training_site-custom-filter-save</t>
+  </si>
+  <si>
+    <t>Admin_282</t>
+  </si>
+  <si>
+    <t>@API Admin training_site-custom-filter-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_283</t>
+  </si>
+  <si>
+    <t>@API Admin training_site-custom-filter-save_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_285</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-field-cloumn-hide and show_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_286</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-field-cloumn-hide and show_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_288</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-pagination_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_289</t>
+  </si>
+  <si>
+    <t>@API Admin training_sites-pagination_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_290</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the deactivate_training_site</t>
+  </si>
+  <si>
+    <t>Admin_291</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for deactivate_training_site</t>
+  </si>
+  <si>
+    <t>Admin_293</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the activate_training_site</t>
+  </si>
+  <si>
+    <t>Admin_294</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for activate_training_site</t>
+  </si>
+  <si>
+    <t>Admin_296</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_site-delete</t>
+  </si>
+  <si>
+    <t>Admin_297</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for training_site-delete</t>
+  </si>
+  <si>
+    <t>Admin_299</t>
+  </si>
+  <si>
+    <t>@API Admin_save-grade-scale</t>
+  </si>
+  <si>
+    <t>Admin_300</t>
+  </si>
+  <si>
+    <t>@API Admin save-grade-scale_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_301</t>
+  </si>
+  <si>
+    <t>@API Admin save-grade-scale_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_314</t>
+  </si>
+  <si>
+    <t>@API Admin_grade-scale-search</t>
+  </si>
+  <si>
+    <t>Admin_315</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_316</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_302</t>
+  </si>
+  <si>
+    <t>@API Admin_grade-scale-edit-form</t>
+  </si>
+  <si>
+    <t>Admin_303</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-edit-form_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_304</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-edit-form_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_305</t>
+  </si>
+  <si>
+    <t>Admin_306</t>
+  </si>
+  <si>
+    <t>Admin_307</t>
+  </si>
+  <si>
+    <t>Admin_308</t>
+  </si>
+  <si>
+    <t>@API Admin_grade-scale-list</t>
+  </si>
+  <si>
+    <t>Admin_309</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-list_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_310</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-list_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_311</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the grade-scale-filters</t>
+  </si>
+  <si>
+    <t>Admin_312</t>
+  </si>
+  <si>
+    <t>@API Endpoint validation for grade-scale-filters</t>
+  </si>
+  <si>
+    <t>Admin_317</t>
+  </si>
+  <si>
+    <t>@API Admin_grade-scale-filter-search</t>
+  </si>
+  <si>
+    <t>Admin_318</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-filter-search_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_319</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-filter-search_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_320</t>
+  </si>
+  <si>
+    <t>@API Admin_grade-scale-custom-filter-save</t>
+  </si>
+  <si>
+    <t>Admin_321</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-custom-filter-save_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_322</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-custom-filter-save_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_323</t>
+  </si>
+  <si>
+    <t>@API Admin_grade-scale-field-column-hide</t>
+  </si>
+  <si>
+    <t>Admin_324</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-field-column-hide_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_325</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-field-column-hide_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_326</t>
+  </si>
+  <si>
+    <t>@API Admin_grade-scale-pagination</t>
+  </si>
+  <si>
+    <t>Admin_327</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-pagination_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_328</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-pagination_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_329</t>
+  </si>
+  <si>
+    <t>@API Admin_duplicate-grade-scale</t>
+  </si>
+  <si>
+    <t>Admin_330</t>
+  </si>
+  <si>
+    <t>@API Admin duplicate-grade-scale_validation of incorrect HTTP method</t>
+  </si>
+  <si>
+    <t>Admin_331</t>
+  </si>
+  <si>
+    <t>@API Admin duplicate-grade-scale_validation of invalid endpoint.</t>
+  </si>
+  <si>
+    <t>Admin_332</t>
+  </si>
+  <si>
+    <t>@API Admin duplicate-grade-scale_validation of invalid grade scale id</t>
+  </si>
+  <si>
+    <t>Admin_522</t>
+  </si>
+  <si>
+    <t>@API Admin add the user and save_validate invalid_userId</t>
+  </si>
+  <si>
+    <t>Admin_525</t>
+  </si>
+  <si>
+    <t>@API Admin_roles-list-search_empty access token</t>
+  </si>
+  <si>
+    <t>Admin_526</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the user-activities-filter_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_527</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the email-template-edit-form_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_528</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the email-template-create-form_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_529</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the email-template-filter-list_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_530</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the duplicate-dashboard_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_531</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the delete-dashboard_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_532</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the chat-settings-form_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_533</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_centre-form_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_534</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_centre-edit-form_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_535</t>
+  </si>
+  <si>
+    <t>@API Admin fetch the training_centres-filters_invalid access token</t>
+  </si>
+  <si>
+    <t>Admin_520</t>
+  </si>
+  <si>
+    <t>@API Admin add the user-save_empty username,email and phone</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>AL_001Zz</t>
+  </si>
+  <si>
+    <t>Admin_521</t>
+  </si>
+  <si>
+    <t>@API Admin add the user and save_empty first_name</t>
+  </si>
+  <si>
+    <t>AL_001Zy</t>
+  </si>
+  <si>
+    <t>Admin_523</t>
+  </si>
+  <si>
+    <t>@API Admin_role-save_empty name</t>
+  </si>
+  <si>
+    <t>AL_001Zxa</t>
+  </si>
+  <si>
+    <t>Admin_524</t>
+  </si>
+  <si>
+    <t>@API Admin_roles-list-search_invalid name</t>
+  </si>
+  <si>
+    <t>AL_001Zx</t>
+  </si>
+  <si>
+    <t>Admin_313</t>
+  </si>
+  <si>
+    <t>@API Admin grade-scale-filters-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zw</t>
+  </si>
+  <si>
+    <t>Admin_298</t>
+  </si>
+  <si>
+    <t>@API Admin training_site-delete-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zv</t>
+  </si>
+  <si>
+    <t>Admin_295</t>
+  </si>
+  <si>
+    <t>@API Admin activate_training_site-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zu</t>
+  </si>
+  <si>
+    <t>Admin_292</t>
+  </si>
+  <si>
+    <t>@API Admin deactivate_training_site-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zt</t>
+  </si>
+  <si>
+    <t>Admin_287</t>
+  </si>
+  <si>
+    <t>@API Admin_training_sites-pagination</t>
+  </si>
+  <si>
+    <t>AL_001Zs</t>
+  </si>
+  <si>
+    <t>Admin_284</t>
+  </si>
+  <si>
+    <t>@API Admin_training_sites-field-cloumn-hide and show</t>
+  </si>
+  <si>
+    <t>AL_001Zr</t>
+  </si>
+  <si>
+    <t>Admin_278</t>
+  </si>
+  <si>
+    <t>@API Admin_training_sites-filter-search</t>
+  </si>
+  <si>
+    <t>AL_001Zq</t>
+  </si>
+  <si>
+    <t>Admin_275</t>
+  </si>
+  <si>
+    <t>@API Admin_training_sites-search</t>
+  </si>
+  <si>
+    <t>AL_001Zp</t>
+  </si>
+  <si>
+    <t>Admin_271</t>
+  </si>
+  <si>
+    <t>@API Admin training_site-edit-form-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zo</t>
+  </si>
+  <si>
+    <t>Admin_265</t>
+  </si>
+  <si>
+    <t>@API Admin training_site-form-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zn</t>
+  </si>
+  <si>
+    <t>Admin_262</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-delete-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zm</t>
+  </si>
+  <si>
+    <t>Admin_259</t>
+  </si>
+  <si>
+    <t>@API Admin activate_training_centre-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zl</t>
+  </si>
+  <si>
+    <t>Admin_256</t>
+  </si>
+  <si>
+    <t>@API Admin deactivate_training_centre-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zk</t>
+  </si>
+  <si>
+    <t>Admin_251</t>
+  </si>
+  <si>
+    <t>@API Admin_training_centres-pagination</t>
+  </si>
+  <si>
+    <t>AL_001Zj</t>
+  </si>
+  <si>
+    <t>Admin_248</t>
+  </si>
+  <si>
+    <t>@API Admin_training_centres-field-column-show and hide</t>
+  </si>
+  <si>
+    <t>AL_001Zi</t>
+  </si>
+  <si>
+    <t>Admin_242</t>
+  </si>
+  <si>
+    <t>@API Admin_training_centres-filter-search</t>
+  </si>
+  <si>
+    <t>AL_001Zh</t>
+  </si>
+  <si>
+    <t>Admin_239</t>
+  </si>
+  <si>
+    <t>@API Admin_training_centres-search</t>
+  </si>
+  <si>
+    <t>AL_001Zg</t>
+  </si>
+  <si>
+    <t>Admin_238</t>
+  </si>
+  <si>
+    <t>@API Admin training_centres-filters-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zf</t>
+  </si>
+  <si>
+    <t>Admin_229</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-edit-form-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Ze</t>
+  </si>
+  <si>
+    <t>Admin_223</t>
+  </si>
+  <si>
+    <t>@API Admin training_centre-form-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zd</t>
+  </si>
+  <si>
+    <t>Admin_217</t>
+  </si>
+  <si>
+    <t>@API Admin chat-settings-form-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zc</t>
+  </si>
+  <si>
+    <t>Admin_214</t>
+  </si>
+  <si>
+    <t>@API Admin delete-dashboard-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Zb</t>
+  </si>
+  <si>
+    <t>Admin_211</t>
+  </si>
+  <si>
+    <t>@API Admin duplicate-dashboard-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Za</t>
+  </si>
+  <si>
+    <t>Admin_203</t>
+  </si>
+  <si>
+    <t>@API Admin dashboard-list-status-change-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Z</t>
+  </si>
+  <si>
+    <t>Admin_189</t>
+  </si>
+  <si>
+    <t>@API Admin dashboard-filter-list-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001Y</t>
+  </si>
+  <si>
+    <t>Admin_154</t>
+  </si>
+  <si>
+    <t>@API Admin email-template-edit-form-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001X</t>
+  </si>
+  <si>
+    <t>Admin_166</t>
+  </si>
+  <si>
+    <t>@API Admin email-template-filter-list-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001W</t>
+  </si>
+  <si>
+    <t>Admin_148</t>
+  </si>
+  <si>
+    <t>@API Admin email-template-create-form-Header field validation - invalid</t>
+  </si>
+  <si>
+    <t>AL_001V</t>
+  </si>
+  <si>
     <t>Admin_094</t>
   </si>
   <si>
     <t>@API Admin security-control-privilage-list-Header field validation - invalid</t>
-  </si>
-  <si>
-    <t>failed</t>
   </si>
   <si>
     <t>AL_001U</t>
@@ -1323,7 +2625,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C168"/>
+  <dimension ref="A1:C403"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2709,15 +4011,15 @@
         <v>248</v>
       </c>
       <c r="C126" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>249</v>
+      </c>
+      <c r="B127" t="s">
         <v>250</v>
-      </c>
-      <c r="B127" t="s">
-        <v>4</v>
       </c>
       <c r="C127" t="s">
         <v>5</v>
@@ -2731,7 +4033,7 @@
         <v>252</v>
       </c>
       <c r="C128" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2739,7 +4041,7 @@
         <v>253</v>
       </c>
       <c r="B129" t="s">
-        <v>4</v>
+        <v>254</v>
       </c>
       <c r="C129" t="s">
         <v>5</v>
@@ -2747,21 +4049,21 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B130" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C130" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>258</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -2769,21 +4071,21 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B132" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C132" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="C133" t="s">
         <v>5</v>
@@ -2791,21 +4093,21 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B134" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C134" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B135" t="s">
-        <v>4</v>
+        <v>266</v>
       </c>
       <c r="C135" t="s">
         <v>5</v>
@@ -2813,21 +4115,21 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B136" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C136" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B137" t="s">
-        <v>4</v>
+        <v>270</v>
       </c>
       <c r="C137" t="s">
         <v>5</v>
@@ -2835,21 +4137,21 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B138" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C138" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>274</v>
       </c>
       <c r="C139" t="s">
         <v>5</v>
@@ -2857,21 +4159,21 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="B140" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C140" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>278</v>
       </c>
       <c r="C141" t="s">
         <v>5</v>
@@ -2879,21 +4181,21 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="B142" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="C142" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>282</v>
       </c>
       <c r="C143" t="s">
         <v>5</v>
@@ -2901,21 +4203,21 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="B144" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="C144" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>286</v>
       </c>
       <c r="C145" t="s">
         <v>5</v>
@@ -2923,21 +4225,21 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="B146" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="C146" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>290</v>
       </c>
       <c r="C147" t="s">
         <v>5</v>
@@ -2945,21 +4247,21 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="B148" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="C148" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="B149" t="s">
-        <v>4</v>
+        <v>294</v>
       </c>
       <c r="C149" t="s">
         <v>5</v>
@@ -2967,21 +4269,21 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="B150" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="C150" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>298</v>
       </c>
       <c r="C151" t="s">
         <v>5</v>
@@ -2989,21 +4291,21 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="B152" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="C152" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
       <c r="B153" t="s">
-        <v>4</v>
+        <v>302</v>
       </c>
       <c r="C153" t="s">
         <v>5</v>
@@ -3011,21 +4313,21 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="B154" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="C154" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="B155" t="s">
-        <v>4</v>
+        <v>306</v>
       </c>
       <c r="C155" t="s">
         <v>5</v>
@@ -3033,21 +4335,21 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B156" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="C156" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>310</v>
       </c>
       <c r="C157" t="s">
         <v>5</v>
@@ -3055,21 +4357,21 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="B158" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="C158" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="B159" t="s">
-        <v>4</v>
+        <v>314</v>
       </c>
       <c r="C159" t="s">
         <v>5</v>
@@ -3077,21 +4379,21 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="B160" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="C160" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="B161" t="s">
-        <v>4</v>
+        <v>318</v>
       </c>
       <c r="C161" t="s">
         <v>5</v>
@@ -3099,21 +4401,21 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="B162" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="C162" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
       <c r="B163" t="s">
-        <v>4</v>
+        <v>322</v>
       </c>
       <c r="C163" t="s">
         <v>5</v>
@@ -3121,21 +4423,21 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="B164" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
       <c r="C164" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="B165" t="s">
-        <v>4</v>
+        <v>326</v>
       </c>
       <c r="C165" t="s">
         <v>5</v>
@@ -3143,21 +4445,21 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="B166" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="C166" t="s">
-        <v>249</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="B167" t="s">
-        <v>4</v>
+        <v>330</v>
       </c>
       <c r="C167" t="s">
         <v>5</v>
@@ -3165,13 +4467,2595 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="B168" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="C168" t="s">
-        <v>249</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>333</v>
+      </c>
+      <c r="B169" t="s">
+        <v>334</v>
+      </c>
+      <c r="C169" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>335</v>
+      </c>
+      <c r="B170" t="s">
+        <v>336</v>
+      </c>
+      <c r="C170" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>337</v>
+      </c>
+      <c r="B171" t="s">
+        <v>338</v>
+      </c>
+      <c r="C171" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>339</v>
+      </c>
+      <c r="B172" t="s">
+        <v>340</v>
+      </c>
+      <c r="C172" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>341</v>
+      </c>
+      <c r="B173" t="s">
+        <v>342</v>
+      </c>
+      <c r="C173" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>343</v>
+      </c>
+      <c r="B174" t="s">
+        <v>344</v>
+      </c>
+      <c r="C174" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>345</v>
+      </c>
+      <c r="B175" t="s">
+        <v>346</v>
+      </c>
+      <c r="C175" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>347</v>
+      </c>
+      <c r="B176" t="s">
+        <v>348</v>
+      </c>
+      <c r="C176" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>349</v>
+      </c>
+      <c r="B177" t="s">
+        <v>350</v>
+      </c>
+      <c r="C177" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>351</v>
+      </c>
+      <c r="B178" t="s">
+        <v>352</v>
+      </c>
+      <c r="C178" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>353</v>
+      </c>
+      <c r="B179" t="s">
+        <v>354</v>
+      </c>
+      <c r="C179" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>355</v>
+      </c>
+      <c r="C180" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>356</v>
+      </c>
+      <c r="B181" t="s">
+        <v>357</v>
+      </c>
+      <c r="C181" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>358</v>
+      </c>
+      <c r="B182" t="s">
+        <v>359</v>
+      </c>
+      <c r="C182" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>360</v>
+      </c>
+      <c r="B183" t="s">
+        <v>361</v>
+      </c>
+      <c r="C183" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>362</v>
+      </c>
+      <c r="B184" t="s">
+        <v>363</v>
+      </c>
+      <c r="C184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>364</v>
+      </c>
+      <c r="B185" t="s">
+        <v>365</v>
+      </c>
+      <c r="C185" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>366</v>
+      </c>
+      <c r="B186" t="s">
+        <v>367</v>
+      </c>
+      <c r="C186" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>368</v>
+      </c>
+      <c r="B187" t="s">
+        <v>369</v>
+      </c>
+      <c r="C187" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>370</v>
+      </c>
+      <c r="B188" t="s">
+        <v>371</v>
+      </c>
+      <c r="C188" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>372</v>
+      </c>
+      <c r="B189" t="s">
+        <v>373</v>
+      </c>
+      <c r="C189" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>374</v>
+      </c>
+      <c r="B190" t="s">
+        <v>375</v>
+      </c>
+      <c r="C190" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>376</v>
+      </c>
+      <c r="B191" t="s">
+        <v>377</v>
+      </c>
+      <c r="C191" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>378</v>
+      </c>
+      <c r="B192" t="s">
+        <v>379</v>
+      </c>
+      <c r="C192" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>380</v>
+      </c>
+      <c r="B193" t="s">
+        <v>381</v>
+      </c>
+      <c r="C193" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>382</v>
+      </c>
+      <c r="B194" t="s">
+        <v>383</v>
+      </c>
+      <c r="C194" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>384</v>
+      </c>
+      <c r="B195" t="s">
+        <v>385</v>
+      </c>
+      <c r="C195" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>386</v>
+      </c>
+      <c r="B196" t="s">
+        <v>387</v>
+      </c>
+      <c r="C196" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>388</v>
+      </c>
+      <c r="B197" t="s">
+        <v>389</v>
+      </c>
+      <c r="C197" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>390</v>
+      </c>
+      <c r="B198" t="s">
+        <v>391</v>
+      </c>
+      <c r="C198" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>392</v>
+      </c>
+      <c r="B199" t="s">
+        <v>393</v>
+      </c>
+      <c r="C199" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>394</v>
+      </c>
+      <c r="B200" t="s">
+        <v>395</v>
+      </c>
+      <c r="C200" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>396</v>
+      </c>
+      <c r="B201" t="s">
+        <v>397</v>
+      </c>
+      <c r="C201" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>398</v>
+      </c>
+      <c r="B202" t="s">
+        <v>399</v>
+      </c>
+      <c r="C202" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>400</v>
+      </c>
+      <c r="B203" t="s">
+        <v>401</v>
+      </c>
+      <c r="C203" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>402</v>
+      </c>
+      <c r="B204" t="s">
+        <v>403</v>
+      </c>
+      <c r="C204" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>404</v>
+      </c>
+      <c r="B205" t="s">
+        <v>405</v>
+      </c>
+      <c r="C205" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>406</v>
+      </c>
+      <c r="B206" t="s">
+        <v>407</v>
+      </c>
+      <c r="C206" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>408</v>
+      </c>
+      <c r="B207" t="s">
+        <v>409</v>
+      </c>
+      <c r="C207" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>410</v>
+      </c>
+      <c r="B208" t="s">
+        <v>411</v>
+      </c>
+      <c r="C208" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>412</v>
+      </c>
+      <c r="B209" t="s">
+        <v>413</v>
+      </c>
+      <c r="C209" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>414</v>
+      </c>
+      <c r="B210" t="s">
+        <v>415</v>
+      </c>
+      <c r="C210" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>416</v>
+      </c>
+      <c r="B211" t="s">
+        <v>417</v>
+      </c>
+      <c r="C211" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>418</v>
+      </c>
+      <c r="B212" t="s">
+        <v>419</v>
+      </c>
+      <c r="C212" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>420</v>
+      </c>
+      <c r="B213" t="s">
+        <v>421</v>
+      </c>
+      <c r="C213" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>422</v>
+      </c>
+      <c r="B214" t="s">
+        <v>423</v>
+      </c>
+      <c r="C214" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>424</v>
+      </c>
+      <c r="B215" t="s">
+        <v>425</v>
+      </c>
+      <c r="C215" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>426</v>
+      </c>
+      <c r="B216" t="s">
+        <v>427</v>
+      </c>
+      <c r="C216" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>428</v>
+      </c>
+      <c r="B217" t="s">
+        <v>429</v>
+      </c>
+      <c r="C217" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>430</v>
+      </c>
+      <c r="B218" t="s">
+        <v>431</v>
+      </c>
+      <c r="C218" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>432</v>
+      </c>
+      <c r="B219" t="s">
+        <v>433</v>
+      </c>
+      <c r="C219" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>434</v>
+      </c>
+      <c r="B220" t="s">
+        <v>435</v>
+      </c>
+      <c r="C220" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>436</v>
+      </c>
+      <c r="B221" t="s">
+        <v>437</v>
+      </c>
+      <c r="C221" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>438</v>
+      </c>
+      <c r="B222" t="s">
+        <v>439</v>
+      </c>
+      <c r="C222" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>440</v>
+      </c>
+      <c r="B223" t="s">
+        <v>441</v>
+      </c>
+      <c r="C223" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>442</v>
+      </c>
+      <c r="B224" t="s">
+        <v>443</v>
+      </c>
+      <c r="C224" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>444</v>
+      </c>
+      <c r="B225" t="s">
+        <v>445</v>
+      </c>
+      <c r="C225" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>446</v>
+      </c>
+      <c r="B226" t="s">
+        <v>447</v>
+      </c>
+      <c r="C226" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>448</v>
+      </c>
+      <c r="B227" t="s">
+        <v>449</v>
+      </c>
+      <c r="C227" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>450</v>
+      </c>
+      <c r="B228" t="s">
+        <v>451</v>
+      </c>
+      <c r="C228" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>452</v>
+      </c>
+      <c r="B229" t="s">
+        <v>453</v>
+      </c>
+      <c r="C229" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>454</v>
+      </c>
+      <c r="B230" t="s">
+        <v>455</v>
+      </c>
+      <c r="C230" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>456</v>
+      </c>
+      <c r="B231" t="s">
+        <v>457</v>
+      </c>
+      <c r="C231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>458</v>
+      </c>
+      <c r="B232" t="s">
+        <v>459</v>
+      </c>
+      <c r="C232" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>460</v>
+      </c>
+      <c r="B233" t="s">
+        <v>461</v>
+      </c>
+      <c r="C233" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>462</v>
+      </c>
+      <c r="B234" t="s">
+        <v>463</v>
+      </c>
+      <c r="C234" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>464</v>
+      </c>
+      <c r="B235" t="s">
+        <v>465</v>
+      </c>
+      <c r="C235" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>466</v>
+      </c>
+      <c r="B236" t="s">
+        <v>467</v>
+      </c>
+      <c r="C236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>468</v>
+      </c>
+      <c r="B237" t="s">
+        <v>469</v>
+      </c>
+      <c r="C237" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>470</v>
+      </c>
+      <c r="B238" t="s">
+        <v>471</v>
+      </c>
+      <c r="C238" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>472</v>
+      </c>
+      <c r="B239" t="s">
+        <v>473</v>
+      </c>
+      <c r="C239" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>474</v>
+      </c>
+      <c r="B240" t="s">
+        <v>475</v>
+      </c>
+      <c r="C240" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>476</v>
+      </c>
+      <c r="B241" t="s">
+        <v>477</v>
+      </c>
+      <c r="C241" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>478</v>
+      </c>
+      <c r="B242" t="s">
+        <v>479</v>
+      </c>
+      <c r="C242" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>480</v>
+      </c>
+      <c r="B243" t="s">
+        <v>481</v>
+      </c>
+      <c r="C243" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>482</v>
+      </c>
+      <c r="B244" t="s">
+        <v>483</v>
+      </c>
+      <c r="C244" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>484</v>
+      </c>
+      <c r="B245" t="s">
+        <v>485</v>
+      </c>
+      <c r="C245" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>486</v>
+      </c>
+      <c r="B246" t="s">
+        <v>487</v>
+      </c>
+      <c r="C246" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>488</v>
+      </c>
+      <c r="B247" t="s">
+        <v>489</v>
+      </c>
+      <c r="C247" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>490</v>
+      </c>
+      <c r="B248" t="s">
+        <v>491</v>
+      </c>
+      <c r="C248" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>492</v>
+      </c>
+      <c r="B249" t="s">
+        <v>493</v>
+      </c>
+      <c r="C249" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>494</v>
+      </c>
+      <c r="B250" t="s">
+        <v>495</v>
+      </c>
+      <c r="C250" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>496</v>
+      </c>
+      <c r="B251" t="s">
+        <v>497</v>
+      </c>
+      <c r="C251" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>498</v>
+      </c>
+      <c r="B252" t="s">
+        <v>499</v>
+      </c>
+      <c r="C252" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>500</v>
+      </c>
+      <c r="B253" t="s">
+        <v>501</v>
+      </c>
+      <c r="C253" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>502</v>
+      </c>
+      <c r="B254" t="s">
+        <v>503</v>
+      </c>
+      <c r="C254" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>504</v>
+      </c>
+      <c r="B255" t="s">
+        <v>505</v>
+      </c>
+      <c r="C255" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>506</v>
+      </c>
+      <c r="B256" t="s">
+        <v>507</v>
+      </c>
+      <c r="C256" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>508</v>
+      </c>
+      <c r="B257" t="s">
+        <v>509</v>
+      </c>
+      <c r="C257" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>510</v>
+      </c>
+      <c r="B258" t="s">
+        <v>511</v>
+      </c>
+      <c r="C258" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>512</v>
+      </c>
+      <c r="B259" t="s">
+        <v>513</v>
+      </c>
+      <c r="C259" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>514</v>
+      </c>
+      <c r="B260" t="s">
+        <v>515</v>
+      </c>
+      <c r="C260" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>516</v>
+      </c>
+      <c r="B261" t="s">
+        <v>499</v>
+      </c>
+      <c r="C261" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>517</v>
+      </c>
+      <c r="B262" t="s">
+        <v>501</v>
+      </c>
+      <c r="C262" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>518</v>
+      </c>
+      <c r="B263" t="s">
+        <v>503</v>
+      </c>
+      <c r="C263" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>519</v>
+      </c>
+      <c r="B264" t="s">
+        <v>520</v>
+      </c>
+      <c r="C264" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>521</v>
+      </c>
+      <c r="B265" t="s">
+        <v>522</v>
+      </c>
+      <c r="C265" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>523</v>
+      </c>
+      <c r="B266" t="s">
+        <v>524</v>
+      </c>
+      <c r="C266" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>525</v>
+      </c>
+      <c r="B267" t="s">
+        <v>526</v>
+      </c>
+      <c r="C267" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>527</v>
+      </c>
+      <c r="B268" t="s">
+        <v>528</v>
+      </c>
+      <c r="C268" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>529</v>
+      </c>
+      <c r="B269" t="s">
+        <v>530</v>
+      </c>
+      <c r="C269" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>531</v>
+      </c>
+      <c r="B270" t="s">
+        <v>532</v>
+      </c>
+      <c r="C270" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>533</v>
+      </c>
+      <c r="B271" t="s">
+        <v>534</v>
+      </c>
+      <c r="C271" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>535</v>
+      </c>
+      <c r="B272" t="s">
+        <v>536</v>
+      </c>
+      <c r="C272" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>537</v>
+      </c>
+      <c r="B273" t="s">
+        <v>538</v>
+      </c>
+      <c r="C273" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>539</v>
+      </c>
+      <c r="B274" t="s">
+        <v>540</v>
+      </c>
+      <c r="C274" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>541</v>
+      </c>
+      <c r="B275" t="s">
+        <v>542</v>
+      </c>
+      <c r="C275" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>543</v>
+      </c>
+      <c r="B276" t="s">
+        <v>544</v>
+      </c>
+      <c r="C276" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>545</v>
+      </c>
+      <c r="B277" t="s">
+        <v>546</v>
+      </c>
+      <c r="C277" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>547</v>
+      </c>
+      <c r="B278" t="s">
+        <v>548</v>
+      </c>
+      <c r="C278" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>549</v>
+      </c>
+      <c r="B279" t="s">
+        <v>550</v>
+      </c>
+      <c r="C279" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>551</v>
+      </c>
+      <c r="B280" t="s">
+        <v>552</v>
+      </c>
+      <c r="C280" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>553</v>
+      </c>
+      <c r="B281" t="s">
+        <v>554</v>
+      </c>
+      <c r="C281" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>555</v>
+      </c>
+      <c r="B282" t="s">
+        <v>556</v>
+      </c>
+      <c r="C282" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>557</v>
+      </c>
+      <c r="B283" t="s">
+        <v>558</v>
+      </c>
+      <c r="C283" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>559</v>
+      </c>
+      <c r="B284" t="s">
+        <v>560</v>
+      </c>
+      <c r="C284" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>561</v>
+      </c>
+      <c r="B285" t="s">
+        <v>562</v>
+      </c>
+      <c r="C285" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>563</v>
+      </c>
+      <c r="B286" t="s">
+        <v>564</v>
+      </c>
+      <c r="C286" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>565</v>
+      </c>
+      <c r="B287" t="s">
+        <v>566</v>
+      </c>
+      <c r="C287" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>567</v>
+      </c>
+      <c r="B288" t="s">
+        <v>568</v>
+      </c>
+      <c r="C288" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>569</v>
+      </c>
+      <c r="B289" t="s">
+        <v>570</v>
+      </c>
+      <c r="C289" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>571</v>
+      </c>
+      <c r="B290" t="s">
+        <v>572</v>
+      </c>
+      <c r="C290" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>573</v>
+      </c>
+      <c r="B291" t="s">
+        <v>574</v>
+      </c>
+      <c r="C291" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>575</v>
+      </c>
+      <c r="B292" t="s">
+        <v>576</v>
+      </c>
+      <c r="C292" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>577</v>
+      </c>
+      <c r="B293" t="s">
+        <v>578</v>
+      </c>
+      <c r="C293" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>579</v>
+      </c>
+      <c r="B294" t="s">
+        <v>580</v>
+      </c>
+      <c r="C294" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>581</v>
+      </c>
+      <c r="B295" t="s">
+        <v>582</v>
+      </c>
+      <c r="C295" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>583</v>
+      </c>
+      <c r="B296" t="s">
+        <v>584</v>
+      </c>
+      <c r="C296" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>585</v>
+      </c>
+      <c r="B297" t="s">
+        <v>586</v>
+      </c>
+      <c r="C297" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>588</v>
+      </c>
+      <c r="B298" t="s">
+        <v>4</v>
+      </c>
+      <c r="C298" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>589</v>
+      </c>
+      <c r="B299" t="s">
+        <v>590</v>
+      </c>
+      <c r="C299" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>591</v>
+      </c>
+      <c r="B300" t="s">
+        <v>4</v>
+      </c>
+      <c r="C300" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>592</v>
+      </c>
+      <c r="B301" t="s">
+        <v>593</v>
+      </c>
+      <c r="C301" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>594</v>
+      </c>
+      <c r="B302" t="s">
+        <v>4</v>
+      </c>
+      <c r="C302" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>595</v>
+      </c>
+      <c r="B303" t="s">
+        <v>596</v>
+      </c>
+      <c r="C303" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>597</v>
+      </c>
+      <c r="B304" t="s">
+        <v>4</v>
+      </c>
+      <c r="C304" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>598</v>
+      </c>
+      <c r="B305" t="s">
+        <v>599</v>
+      </c>
+      <c r="C305" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>600</v>
+      </c>
+      <c r="B306" t="s">
+        <v>4</v>
+      </c>
+      <c r="C306" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>601</v>
+      </c>
+      <c r="B307" t="s">
+        <v>602</v>
+      </c>
+      <c r="C307" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>603</v>
+      </c>
+      <c r="B308" t="s">
+        <v>4</v>
+      </c>
+      <c r="C308" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>604</v>
+      </c>
+      <c r="B309" t="s">
+        <v>605</v>
+      </c>
+      <c r="C309" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>606</v>
+      </c>
+      <c r="B310" t="s">
+        <v>4</v>
+      </c>
+      <c r="C310" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>607</v>
+      </c>
+      <c r="B311" t="s">
+        <v>608</v>
+      </c>
+      <c r="C311" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>609</v>
+      </c>
+      <c r="B312" t="s">
+        <v>4</v>
+      </c>
+      <c r="C312" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>610</v>
+      </c>
+      <c r="B313" t="s">
+        <v>611</v>
+      </c>
+      <c r="C313" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>612</v>
+      </c>
+      <c r="B314" t="s">
+        <v>4</v>
+      </c>
+      <c r="C314" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>613</v>
+      </c>
+      <c r="B315" t="s">
+        <v>614</v>
+      </c>
+      <c r="C315" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>615</v>
+      </c>
+      <c r="B316" t="s">
+        <v>4</v>
+      </c>
+      <c r="C316" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>616</v>
+      </c>
+      <c r="B317" t="s">
+        <v>617</v>
+      </c>
+      <c r="C317" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>618</v>
+      </c>
+      <c r="B318" t="s">
+        <v>4</v>
+      </c>
+      <c r="C318" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>619</v>
+      </c>
+      <c r="B319" t="s">
+        <v>620</v>
+      </c>
+      <c r="C319" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>621</v>
+      </c>
+      <c r="B320" t="s">
+        <v>4</v>
+      </c>
+      <c r="C320" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>622</v>
+      </c>
+      <c r="B321" t="s">
+        <v>623</v>
+      </c>
+      <c r="C321" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>624</v>
+      </c>
+      <c r="B322" t="s">
+        <v>4</v>
+      </c>
+      <c r="C322" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>625</v>
+      </c>
+      <c r="B323" t="s">
+        <v>626</v>
+      </c>
+      <c r="C323" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>627</v>
+      </c>
+      <c r="B324" t="s">
+        <v>4</v>
+      </c>
+      <c r="C324" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>628</v>
+      </c>
+      <c r="B325" t="s">
+        <v>629</v>
+      </c>
+      <c r="C325" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>630</v>
+      </c>
+      <c r="B326" t="s">
+        <v>4</v>
+      </c>
+      <c r="C326" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>631</v>
+      </c>
+      <c r="B327" t="s">
+        <v>632</v>
+      </c>
+      <c r="C327" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>633</v>
+      </c>
+      <c r="B328" t="s">
+        <v>4</v>
+      </c>
+      <c r="C328" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>634</v>
+      </c>
+      <c r="B329" t="s">
+        <v>635</v>
+      </c>
+      <c r="C329" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>636</v>
+      </c>
+      <c r="B330" t="s">
+        <v>4</v>
+      </c>
+      <c r="C330" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>637</v>
+      </c>
+      <c r="B331" t="s">
+        <v>638</v>
+      </c>
+      <c r="C331" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>639</v>
+      </c>
+      <c r="B332" t="s">
+        <v>4</v>
+      </c>
+      <c r="C332" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>640</v>
+      </c>
+      <c r="B333" t="s">
+        <v>641</v>
+      </c>
+      <c r="C333" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>642</v>
+      </c>
+      <c r="B334" t="s">
+        <v>4</v>
+      </c>
+      <c r="C334" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>643</v>
+      </c>
+      <c r="B335" t="s">
+        <v>644</v>
+      </c>
+      <c r="C335" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>645</v>
+      </c>
+      <c r="B336" t="s">
+        <v>4</v>
+      </c>
+      <c r="C336" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>646</v>
+      </c>
+      <c r="B337" t="s">
+        <v>647</v>
+      </c>
+      <c r="C337" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>648</v>
+      </c>
+      <c r="B338" t="s">
+        <v>4</v>
+      </c>
+      <c r="C338" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>649</v>
+      </c>
+      <c r="B339" t="s">
+        <v>650</v>
+      </c>
+      <c r="C339" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>651</v>
+      </c>
+      <c r="B340" t="s">
+        <v>4</v>
+      </c>
+      <c r="C340" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>652</v>
+      </c>
+      <c r="B341" t="s">
+        <v>653</v>
+      </c>
+      <c r="C341" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>654</v>
+      </c>
+      <c r="B342" t="s">
+        <v>4</v>
+      </c>
+      <c r="C342" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>655</v>
+      </c>
+      <c r="B343" t="s">
+        <v>656</v>
+      </c>
+      <c r="C343" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>657</v>
+      </c>
+      <c r="B344" t="s">
+        <v>4</v>
+      </c>
+      <c r="C344" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>658</v>
+      </c>
+      <c r="B345" t="s">
+        <v>659</v>
+      </c>
+      <c r="C345" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>660</v>
+      </c>
+      <c r="B346" t="s">
+        <v>4</v>
+      </c>
+      <c r="C346" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>661</v>
+      </c>
+      <c r="B347" t="s">
+        <v>662</v>
+      </c>
+      <c r="C347" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>663</v>
+      </c>
+      <c r="B348" t="s">
+        <v>4</v>
+      </c>
+      <c r="C348" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>664</v>
+      </c>
+      <c r="B349" t="s">
+        <v>665</v>
+      </c>
+      <c r="C349" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>666</v>
+      </c>
+      <c r="B350" t="s">
+        <v>4</v>
+      </c>
+      <c r="C350" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>667</v>
+      </c>
+      <c r="B351" t="s">
+        <v>668</v>
+      </c>
+      <c r="C351" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>669</v>
+      </c>
+      <c r="B352" t="s">
+        <v>4</v>
+      </c>
+      <c r="C352" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>670</v>
+      </c>
+      <c r="B353" t="s">
+        <v>671</v>
+      </c>
+      <c r="C353" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>672</v>
+      </c>
+      <c r="B354" t="s">
+        <v>4</v>
+      </c>
+      <c r="C354" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>673</v>
+      </c>
+      <c r="B355" t="s">
+        <v>674</v>
+      </c>
+      <c r="C355" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>675</v>
+      </c>
+      <c r="B356" t="s">
+        <v>4</v>
+      </c>
+      <c r="C356" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>676</v>
+      </c>
+      <c r="B357" t="s">
+        <v>677</v>
+      </c>
+      <c r="C357" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>678</v>
+      </c>
+      <c r="B358" t="s">
+        <v>4</v>
+      </c>
+      <c r="C358" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>679</v>
+      </c>
+      <c r="B359" t="s">
+        <v>680</v>
+      </c>
+      <c r="C359" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>681</v>
+      </c>
+      <c r="B360" t="s">
+        <v>4</v>
+      </c>
+      <c r="C360" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>682</v>
+      </c>
+      <c r="B361" t="s">
+        <v>683</v>
+      </c>
+      <c r="C361" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>684</v>
+      </c>
+      <c r="B362" t="s">
+        <v>4</v>
+      </c>
+      <c r="C362" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>685</v>
+      </c>
+      <c r="B363" t="s">
+        <v>686</v>
+      </c>
+      <c r="C363" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>687</v>
+      </c>
+      <c r="B364" t="s">
+        <v>4</v>
+      </c>
+      <c r="C364" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>688</v>
+      </c>
+      <c r="B365" t="s">
+        <v>689</v>
+      </c>
+      <c r="C365" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>690</v>
+      </c>
+      <c r="B366" t="s">
+        <v>4</v>
+      </c>
+      <c r="C366" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>691</v>
+      </c>
+      <c r="B367" t="s">
+        <v>692</v>
+      </c>
+      <c r="C367" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>693</v>
+      </c>
+      <c r="B368" t="s">
+        <v>4</v>
+      </c>
+      <c r="C368" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>694</v>
+      </c>
+      <c r="B369" t="s">
+        <v>695</v>
+      </c>
+      <c r="C369" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>696</v>
+      </c>
+      <c r="B370" t="s">
+        <v>4</v>
+      </c>
+      <c r="C370" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>697</v>
+      </c>
+      <c r="B371" t="s">
+        <v>698</v>
+      </c>
+      <c r="C371" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>699</v>
+      </c>
+      <c r="B372" t="s">
+        <v>4</v>
+      </c>
+      <c r="C372" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>700</v>
+      </c>
+      <c r="B373" t="s">
+        <v>701</v>
+      </c>
+      <c r="C373" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>702</v>
+      </c>
+      <c r="B374" t="s">
+        <v>4</v>
+      </c>
+      <c r="C374" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>703</v>
+      </c>
+      <c r="B375" t="s">
+        <v>704</v>
+      </c>
+      <c r="C375" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>705</v>
+      </c>
+      <c r="B376" t="s">
+        <v>4</v>
+      </c>
+      <c r="C376" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>706</v>
+      </c>
+      <c r="B377" t="s">
+        <v>707</v>
+      </c>
+      <c r="C377" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>708</v>
+      </c>
+      <c r="B378" t="s">
+        <v>4</v>
+      </c>
+      <c r="C378" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>709</v>
+      </c>
+      <c r="B379" t="s">
+        <v>710</v>
+      </c>
+      <c r="C379" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>711</v>
+      </c>
+      <c r="B380" t="s">
+        <v>4</v>
+      </c>
+      <c r="C380" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>712</v>
+      </c>
+      <c r="B381" t="s">
+        <v>713</v>
+      </c>
+      <c r="C381" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>714</v>
+      </c>
+      <c r="B382" t="s">
+        <v>4</v>
+      </c>
+      <c r="C382" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>715</v>
+      </c>
+      <c r="B383" t="s">
+        <v>716</v>
+      </c>
+      <c r="C383" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>717</v>
+      </c>
+      <c r="B384" t="s">
+        <v>4</v>
+      </c>
+      <c r="C384" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>718</v>
+      </c>
+      <c r="B385" t="s">
+        <v>719</v>
+      </c>
+      <c r="C385" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>720</v>
+      </c>
+      <c r="B386" t="s">
+        <v>4</v>
+      </c>
+      <c r="C386" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>721</v>
+      </c>
+      <c r="B387" t="s">
+        <v>719</v>
+      </c>
+      <c r="C387" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>722</v>
+      </c>
+      <c r="B388" t="s">
+        <v>4</v>
+      </c>
+      <c r="C388" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>723</v>
+      </c>
+      <c r="B389" t="s">
+        <v>724</v>
+      </c>
+      <c r="C389" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>725</v>
+      </c>
+      <c r="B390" t="s">
+        <v>4</v>
+      </c>
+      <c r="C390" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>726</v>
+      </c>
+      <c r="B391" t="s">
+        <v>727</v>
+      </c>
+      <c r="C391" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>728</v>
+      </c>
+      <c r="B392" t="s">
+        <v>4</v>
+      </c>
+      <c r="C392" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>729</v>
+      </c>
+      <c r="B393" t="s">
+        <v>730</v>
+      </c>
+      <c r="C393" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>731</v>
+      </c>
+      <c r="B394" t="s">
+        <v>4</v>
+      </c>
+      <c r="C394" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>732</v>
+      </c>
+      <c r="B395" t="s">
+        <v>733</v>
+      </c>
+      <c r="C395" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>734</v>
+      </c>
+      <c r="B396" t="s">
+        <v>4</v>
+      </c>
+      <c r="C396" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>735</v>
+      </c>
+      <c r="B397" t="s">
+        <v>736</v>
+      </c>
+      <c r="C397" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>737</v>
+      </c>
+      <c r="B398" t="s">
+        <v>4</v>
+      </c>
+      <c r="C398" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>738</v>
+      </c>
+      <c r="B399" t="s">
+        <v>739</v>
+      </c>
+      <c r="C399" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>740</v>
+      </c>
+      <c r="B400" t="s">
+        <v>4</v>
+      </c>
+      <c r="C400" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>741</v>
+      </c>
+      <c r="B401" t="s">
+        <v>742</v>
+      </c>
+      <c r="C401" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>743</v>
+      </c>
+      <c r="B402" t="s">
+        <v>4</v>
+      </c>
+      <c r="C402" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>744</v>
+      </c>
+      <c r="B403" t="s">
+        <v>745</v>
+      </c>
+      <c r="C403" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>